<commit_message>
add necessary imports and make the code runnable
</commit_message>
<xml_diff>
--- a/output/cai-immunofluorescence-rewritten.xlsx
+++ b/output/cai-immunofluorescence-rewritten.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fatho\Dropbox\Code\Python\docx-sop-parser\output\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D7D370-4B88-4B78-A931-DB86E047E0DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32280" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -187,8 +181,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,14 +219,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -279,7 +265,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -311,27 +297,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -363,24 +331,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -556,19 +506,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="58.6328125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -579,7 +524,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -590,7 +535,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -601,7 +546,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -612,7 +557,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -623,7 +568,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -634,7 +579,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -645,7 +590,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -656,7 +601,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>2</v>
       </c>
@@ -667,7 +612,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>2</v>
       </c>
@@ -678,7 +623,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>2</v>
       </c>
@@ -689,7 +634,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>2</v>
       </c>
@@ -700,7 +645,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>2</v>
       </c>
@@ -711,7 +656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>2</v>
       </c>
@@ -722,7 +667,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>2</v>
       </c>
@@ -733,7 +678,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>2</v>
       </c>
@@ -744,7 +689,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>2</v>
       </c>
@@ -755,7 +700,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>2</v>
       </c>
@@ -766,7 +711,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>2</v>
       </c>
@@ -777,7 +722,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>3</v>
       </c>
@@ -788,7 +733,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>3</v>
       </c>
@@ -799,7 +744,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3">
       <c r="A22">
         <v>3</v>
       </c>
@@ -810,7 +755,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3">
       <c r="A23">
         <v>3</v>
       </c>
@@ -821,7 +766,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3">
       <c r="A24">
         <v>3</v>
       </c>
@@ -832,7 +777,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3">
       <c r="A25">
         <v>4</v>
       </c>
@@ -843,7 +788,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3">
       <c r="A26">
         <v>5</v>
       </c>
@@ -854,7 +799,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3">
       <c r="A27">
         <v>5</v>
       </c>
@@ -865,7 +810,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3">
       <c r="A28">
         <v>5</v>
       </c>
@@ -876,7 +821,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3">
       <c r="A29">
         <v>5</v>
       </c>
@@ -887,7 +832,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3">
       <c r="A30">
         <v>5</v>
       </c>
@@ -898,7 +843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3">
       <c r="A31">
         <v>5</v>
       </c>
@@ -909,7 +854,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3">
       <c r="A32">
         <v>5</v>
       </c>
@@ -920,7 +865,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3">
       <c r="A33">
         <v>5</v>
       </c>
@@ -931,7 +876,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3">
       <c r="A34">
         <v>5</v>
       </c>
@@ -942,7 +887,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3">
       <c r="A35">
         <v>5</v>
       </c>
@@ -953,7 +898,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3">
       <c r="A36">
         <v>5</v>
       </c>
@@ -964,7 +909,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3">
       <c r="A37">
         <v>6</v>
       </c>
@@ -975,7 +920,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3">
       <c r="A38">
         <v>6</v>
       </c>
@@ -986,7 +931,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3">
       <c r="A39">
         <v>6</v>
       </c>
@@ -997,7 +942,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3">
       <c r="A40">
         <v>7</v>
       </c>
@@ -1008,7 +953,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3">
       <c r="A41">
         <v>7</v>
       </c>
@@ -1019,7 +964,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3">
       <c r="A42">
         <v>7</v>
       </c>
@@ -1030,7 +975,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3">
       <c r="A43">
         <v>7</v>
       </c>
@@ -1041,7 +986,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3">
       <c r="A44">
         <v>8</v>
       </c>
@@ -1052,7 +997,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3">
       <c r="A45">
         <v>8</v>
       </c>
@@ -1063,7 +1008,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3">
       <c r="A46">
         <v>8</v>
       </c>
@@ -1074,7 +1019,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3">
       <c r="A47">
         <v>8</v>
       </c>
@@ -1085,7 +1030,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3">
       <c r="A48">
         <v>8</v>
       </c>
@@ -1096,7 +1041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3">
       <c r="A49">
         <v>8</v>
       </c>
@@ -1107,7 +1052,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3">
       <c r="A50">
         <v>8</v>
       </c>
@@ -1118,7 +1063,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3">
       <c r="A51">
         <v>8</v>
       </c>
@@ -1129,7 +1074,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3">
       <c r="A52">
         <v>8</v>
       </c>
@@ -1140,7 +1085,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3">
       <c r="A53">
         <v>8</v>
       </c>
@@ -1151,7 +1096,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3">
       <c r="A54">
         <v>8</v>
       </c>
@@ -1162,7 +1107,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3">
       <c r="A55">
         <v>8</v>
       </c>
@@ -1173,7 +1118,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3">
       <c r="A56">
         <v>9</v>
       </c>
@@ -1184,7 +1129,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3">
       <c r="A57">
         <v>9</v>
       </c>
@@ -1195,7 +1140,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3">
       <c r="A58">
         <v>9</v>
       </c>
@@ -1206,7 +1151,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3">
       <c r="A59">
         <v>10</v>
       </c>
@@ -1217,7 +1162,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3">
       <c r="A60">
         <v>10</v>
       </c>
@@ -1228,7 +1173,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3">
       <c r="A61">
         <v>10</v>
       </c>
@@ -1239,7 +1184,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3">
       <c r="A62">
         <v>10</v>
       </c>
@@ -1250,7 +1195,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3">
       <c r="A63">
         <v>10</v>
       </c>
@@ -1261,7 +1206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3">
       <c r="A64">
         <v>10</v>
       </c>
@@ -1272,7 +1217,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3">
       <c r="A65">
         <v>10</v>
       </c>
@@ -1283,7 +1228,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3">
       <c r="A66">
         <v>10</v>
       </c>
@@ -1294,7 +1239,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3">
       <c r="A67">
         <v>10</v>
       </c>
@@ -1305,7 +1250,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3">
       <c r="A68">
         <v>10</v>
       </c>
@@ -1316,7 +1261,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3">
       <c r="A69">
         <v>10</v>
       </c>
@@ -1327,7 +1272,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3">
       <c r="A70">
         <v>10</v>
       </c>
@@ -1338,7 +1283,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3">
       <c r="A71">
         <v>11</v>
       </c>
@@ -1349,7 +1294,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3">
       <c r="A72">
         <v>11</v>
       </c>
@@ -1360,7 +1305,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3">
       <c r="A73">
         <v>11</v>
       </c>
@@ -1371,7 +1316,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3">
       <c r="A74">
         <v>12</v>
       </c>
@@ -1382,7 +1327,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3">
       <c r="A75">
         <v>12</v>
       </c>
@@ -1393,7 +1338,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3">
       <c r="A76">
         <v>12</v>
       </c>
@@ -1404,7 +1349,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3">
       <c r="A77">
         <v>12</v>
       </c>
@@ -1415,7 +1360,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3">
       <c r="A78">
         <v>12</v>
       </c>
@@ -1426,7 +1371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3">
       <c r="A79">
         <v>12</v>
       </c>
@@ -1437,7 +1382,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3">
       <c r="A80">
         <v>12</v>
       </c>
@@ -1448,7 +1393,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3">
       <c r="A81">
         <v>12</v>
       </c>
@@ -1459,7 +1404,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3">
       <c r="A82">
         <v>12</v>
       </c>
@@ -1470,7 +1415,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:3">
       <c r="A83">
         <v>12</v>
       </c>
@@ -1481,7 +1426,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:3">
       <c r="A84">
         <v>12</v>
       </c>
@@ -1492,7 +1437,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:3">
       <c r="A85">
         <v>12</v>
       </c>
@@ -1503,7 +1448,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:3">
       <c r="A86">
         <v>13</v>
       </c>
@@ -1514,7 +1459,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:3">
       <c r="A87">
         <v>13</v>
       </c>
@@ -1525,7 +1470,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:3">
       <c r="A88">
         <v>13</v>
       </c>
@@ -1536,7 +1481,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:3">
       <c r="A89">
         <v>14</v>
       </c>
@@ -1547,7 +1492,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:3">
       <c r="A90">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
recognize orphaned bracket pairs and log accordingly
</commit_message>
<xml_diff>
--- a/output/cai-immunofluorescence-rewritten.xlsx
+++ b/output/cai-immunofluorescence-rewritten.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="45">
   <si>
     <t>STEP NUMBER</t>
   </si>
@@ -149,33 +149,6 @@
   </si>
   <si>
     <t>secondary</t>
-  </si>
-  <si>
-    <t>fluorescent</t>
-  </si>
-  <si>
-    <t>DAPI)</t>
-  </si>
-  <si>
-    <t>mounting</t>
-  </si>
-  <si>
-    <t>mountant</t>
-  </si>
-  <si>
-    <t>ProLong Gold</t>
-  </si>
-  <si>
-    <t>ProLong Diamond</t>
-  </si>
-  <si>
-    <t>polymerization</t>
-  </si>
-  <si>
-    <t>temperature</t>
-  </si>
-  <si>
-    <t>room</t>
   </si>
 </sst>
 </file>
@@ -507,7 +480,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C90"/>
+  <dimension ref="A1:C70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1283,226 +1256,6 @@
         <v>13</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
-      <c r="A71">
-        <v>11</v>
-      </c>
-      <c r="B71" t="s">
-        <v>16</v>
-      </c>
-      <c r="C71" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72">
-        <v>11</v>
-      </c>
-      <c r="B72" t="s">
-        <v>6</v>
-      </c>
-      <c r="C72" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73">
-        <v>11</v>
-      </c>
-      <c r="B73" t="s">
-        <v>45</v>
-      </c>
-      <c r="C73" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74">
-        <v>12</v>
-      </c>
-      <c r="B74" t="s">
-        <v>18</v>
-      </c>
-      <c r="C74" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75">
-        <v>12</v>
-      </c>
-      <c r="B75" t="s">
-        <v>20</v>
-      </c>
-      <c r="C75" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="A76">
-        <v>12</v>
-      </c>
-      <c r="B76" t="s">
-        <v>22</v>
-      </c>
-      <c r="C76" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="A77">
-        <v>12</v>
-      </c>
-      <c r="B77" t="s">
-        <v>24</v>
-      </c>
-      <c r="C77" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="A78">
-        <v>12</v>
-      </c>
-      <c r="B78" t="s">
-        <v>26</v>
-      </c>
-      <c r="C78">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="A79">
-        <v>12</v>
-      </c>
-      <c r="B79" t="s">
-        <v>27</v>
-      </c>
-      <c r="C79">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="A80">
-        <v>12</v>
-      </c>
-      <c r="B80" t="s">
-        <v>28</v>
-      </c>
-      <c r="C80" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="A81">
-        <v>12</v>
-      </c>
-      <c r="B81" t="s">
-        <v>30</v>
-      </c>
-      <c r="C81" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3">
-      <c r="A82">
-        <v>12</v>
-      </c>
-      <c r="B82" t="s">
-        <v>6</v>
-      </c>
-      <c r="C82" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="A83">
-        <v>12</v>
-      </c>
-      <c r="B83" t="s">
-        <v>16</v>
-      </c>
-      <c r="C83" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3">
-      <c r="A84">
-        <v>12</v>
-      </c>
-      <c r="B84" t="s">
-        <v>14</v>
-      </c>
-      <c r="C84" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3">
-      <c r="A85">
-        <v>12</v>
-      </c>
-      <c r="B85" t="s">
-        <v>12</v>
-      </c>
-      <c r="C85" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3">
-      <c r="A86">
-        <v>13</v>
-      </c>
-      <c r="B86" t="s">
-        <v>6</v>
-      </c>
-      <c r="C86" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3">
-      <c r="A87">
-        <v>13</v>
-      </c>
-      <c r="B87" t="s">
-        <v>48</v>
-      </c>
-      <c r="C87" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3">
-      <c r="A88">
-        <v>13</v>
-      </c>
-      <c r="B88" t="s">
-        <v>48</v>
-      </c>
-      <c r="C88" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3">
-      <c r="A89">
-        <v>14</v>
-      </c>
-      <c r="B89" t="s">
-        <v>6</v>
-      </c>
-      <c r="C89" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3">
-      <c r="A90">
-        <v>14</v>
-      </c>
-      <c r="B90" t="s">
-        <v>52</v>
-      </c>
-      <c r="C90" t="s">
-        <v>53</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>